<commit_message>
docs(linea-base-03): corrige errores en la línea base 3
</commit_message>
<xml_diff>
--- a/02 DESARROLLO/SCELS/03 DESARROLLO/DOCS/SCELS-CP-018.xlsx
+++ b/02 DESARROLLO/SCELS/03 DESARROLLO/DOCS/SCELS-CP-018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ara\Desktop\GitHub\BAKATI-GROUP\02 DESARROLLO\SCELS\03 DESARROLLO\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E40055A-1EB4-41AB-B861-B500DE7490D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70674AF8-0E97-42B9-A39C-05CCF458C66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,7 +470,7 @@
     <t>SCELS-PROTO.FIG</t>
   </si>
   <si>
-    <t>SCELS-COD.ZIP</t>
+    <t>SCELS-COD.RAR</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>